<commit_message>
Update In-game context edited.xlsx
</commit_message>
<xml_diff>
--- a/mechanical_turk/HTML_files/In-game context edited.xlsx
+++ b/mechanical_turk/HTML_files/In-game context edited.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Documents\GitHub\ARL\mechanical_turk\HTML_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DCE7DD6-5985-40AA-8D9A-C3D8663291E6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2210D2B0-C234-40BD-94C2-937166B840F1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8520" xr2:uid="{3C25DF8E-F82D-42EE-B09B-A9B128278D29}"/>
   </bookViews>
@@ -33,9 +33,6 @@
     <t xml:space="preserve">Explain that Captain Heist could not make it. You will be leading in his absence </t>
   </si>
   <si>
-    <t>You are running short on time and don't understand why it is necessary to discuss this in private later. You could explain how you feel or just tell him the meeing won't take long.</t>
-  </si>
-  <si>
     <t xml:space="preserve">You don't understand what benefit his method has because he will be spliting up the supplies, so refugees won't be able to get everything at one place. You could directly express this concern or explain again that your plan was to use one aid station with American medics and ask him how his plan is better. </t>
   </si>
   <si>
@@ -88,6 +85,9 @@
   </si>
   <si>
     <t>You want to ask him why his plan calls for setting up two aid stations.</t>
+  </si>
+  <si>
+    <t>You are running short on time and don't understand why it is necessary to discuss this in private later. You could explain how you feel or just tell him the meeting won't take long.</t>
   </si>
 </sst>
 </file>
@@ -569,7 +569,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -583,7 +583,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -591,7 +591,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -607,7 +607,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -615,7 +615,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -623,7 +623,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -631,7 +631,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -639,7 +639,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -647,7 +647,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -655,7 +655,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -663,7 +663,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -671,7 +671,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -679,7 +679,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -687,7 +687,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -695,7 +695,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -703,7 +703,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -711,7 +711,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -719,7 +719,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -727,7 +727,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -735,7 +735,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>